<commit_message>
Updated by adding methods to Edit excel file
</commit_message>
<xml_diff>
--- a/ExcelWriterApp/Excel_With_Styles.xlsx
+++ b/ExcelWriterApp/Excel_With_Styles.xlsx
@@ -194,9 +194,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="#&quot; m&quot;"/>
-    <numFmt numFmtId="165" formatCode="#&quot; ft&quot;"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="#&quot; m&quot;"/>
+    <numFmt numFmtId="166" formatCode="#&quot; ft&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -458,46 +459,46 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="166" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>

</xml_diff>